<commit_message>
P-10 and P-11 completed
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -250,17 +250,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,18 +789,18 @@
       </c>
     </row>
     <row r="12" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
P-12 completed delete list enabled
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="JSEvents" sheetId="1" r:id="rId1"/>
-    <sheet name="allEvents" sheetId="2" r:id="rId2"/>
+    <sheet name="allEvents" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,100 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
-  <si>
-    <t>Event</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>technique</t>
-  </si>
-  <si>
-    <t>Array of cards</t>
-  </si>
-  <si>
-    <t>Var Name in JS</t>
-  </si>
-  <si>
-    <t>takes the input as heading of card and adds a card</t>
-  </si>
-  <si>
-    <t>CardArray</t>
-  </si>
-  <si>
-    <t>Card1</t>
-  </si>
-  <si>
-    <t>card2</t>
-  </si>
-  <si>
-    <t>Card3</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>Array of Objects</t>
-  </si>
-  <si>
-    <t>Heading</t>
-  </si>
-  <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>list of tasks</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>add buttton in card</t>
-  </si>
-  <si>
-    <t>shows the popup to enter the task</t>
-  </si>
-  <si>
-    <t>CSS</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>add button in pop up - 1(add card)</t>
-  </si>
-  <si>
-    <t>add button in pop up - 2(add task to card)</t>
-  </si>
-  <si>
-    <t>takes the input as task name and adds to the card</t>
-  </si>
-  <si>
-    <t>Array of tasks</t>
-  </si>
-  <si>
-    <t>TaskName</t>
-  </si>
-  <si>
-    <t>isMarked</t>
-  </si>
-  <si>
-    <t>input value from add popup-2</t>
-  </si>
-  <si>
-    <t>input value from add popup-1</t>
-  </si>
-  <si>
-    <t>checks if the task is done</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>add item - when user click on this it shows a pop up asking the user about the new list name to be added</t>
   </si>
@@ -194,6 +100,18 @@
   </si>
   <si>
     <t>P-11</t>
+  </si>
+  <si>
+    <t>P-12</t>
+  </si>
+  <si>
+    <t>Delete btn - when user clicks on this it deletes the complete list</t>
+  </si>
+  <si>
+    <t>P-13</t>
+  </si>
+  <si>
+    <t>Use local storage to avoid losing data once page is refreshed</t>
   </si>
 </sst>
 </file>
@@ -223,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -246,17 +164,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -539,176 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L10"/>
+  <dimension ref="C3:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,91 +488,113 @@
   <sheetData>
     <row r="3" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="60" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
P-13 completed(localstorage added) Project Completed Hopefully Final Commit
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -179,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -190,9 +190,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -478,7 +475,7 @@
   <dimension ref="C3:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,10 +580,10 @@
       </c>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>